<commit_message>
Hoàn thành Báo cáo Đồ án chuyên ngành
</commit_message>
<xml_diff>
--- a/Ke-hoach-lam-viec-nhom-21.xlsx
+++ b/Ke-hoach-lam-viec-nhom-21.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - klkaht\Documents\HaUI\File hoc ky VII\Do an chuyen nganh\DACN_Nhom21\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8E88E16-4D73-462A-8422-75719E38A6C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B52648-19C9-4B4A-9129-64A2AE6F1433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="2520" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Kế hoạch" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
   <si>
     <t>Kế hoạch làm việc nhóm</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>Ngày bắt đầu - Start time: 11/09/2024</t>
-  </si>
-  <si>
-    <t>Ngày kết thúc - End date: 18/12/2024</t>
   </si>
   <si>
     <t>Nhóm: 21</t>
@@ -170,9 +167,6 @@
     <t>Tiến hành kiểm thử ứng dụng</t>
   </si>
   <si>
-    <t>On-go</t>
-  </si>
-  <si>
     <t>Phạm Đức Thắng</t>
   </si>
   <si>
@@ -183,6 +177,9 @@
   </si>
   <si>
     <t>Hoàn thiện báo cáo bài tập lớn</t>
+  </si>
+  <si>
+    <t>Ngày kết thúc - End date: 22/12/2024</t>
   </si>
 </sst>
 </file>
@@ -565,8 +562,8 @@
   </sheetPr>
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -610,7 +607,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -670,7 +667,7 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B4" s="21"/>
       <c r="C4" s="21"/>
@@ -700,7 +697,7 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -739,7 +736,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>4</v>
@@ -885,7 +882,7 @@
         <v>10</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="1"/>
@@ -911,7 +908,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="7">
         <v>45564</v>
@@ -922,12 +919,14 @@
       <c r="E10" s="9">
         <v>45575</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" s="9">
+        <v>45575</v>
+      </c>
       <c r="G10" s="8" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="1"/>
@@ -952,7 +951,7 @@
         <v>5</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="7">
         <v>45564</v>
@@ -963,12 +962,14 @@
       <c r="E11" s="9">
         <v>45575</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" s="9">
+        <v>45575</v>
+      </c>
       <c r="G11" s="8" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="1"/>
@@ -993,7 +994,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="7">
         <v>45564</v>
@@ -1004,12 +1005,14 @@
       <c r="E12" s="9">
         <v>45575</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" s="9">
+        <v>45575</v>
+      </c>
       <c r="G12" s="8" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="1"/>
@@ -1034,7 +1037,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="7">
         <v>45564</v>
@@ -1045,12 +1048,14 @@
       <c r="E13" s="9">
         <v>45575</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" s="9">
+        <v>45575</v>
+      </c>
       <c r="G13" s="8" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="1"/>
@@ -1075,7 +1080,7 @@
         <v>8</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="7">
         <v>45564</v>
@@ -1086,12 +1091,14 @@
       <c r="E14" s="9">
         <v>45575</v>
       </c>
-      <c r="F14" s="9"/>
+      <c r="F14" s="9">
+        <v>45575</v>
+      </c>
       <c r="G14" s="8" t="s">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="1"/>
@@ -1122,12 +1129,18 @@
       <c r="C15" s="10">
         <v>45576</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="10">
+        <v>45576</v>
+      </c>
       <c r="E15" s="10">
         <v>45583</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="6"/>
+      <c r="F15" s="10">
+        <v>45583</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H15" s="6" t="s">
         <v>11</v>
       </c>
@@ -1160,12 +1173,18 @@
       <c r="C16" s="10">
         <v>45576</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="10">
+        <v>45576</v>
+      </c>
       <c r="E16" s="10">
         <v>45583</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="6"/>
+      <c r="F16" s="10">
+        <v>45583</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H16" s="6" t="s">
         <v>11</v>
       </c>
@@ -1198,13 +1217,21 @@
       <c r="C17" s="10">
         <v>45576</v>
       </c>
-      <c r="D17" s="10"/>
+      <c r="D17" s="10">
+        <v>45576</v>
+      </c>
       <c r="E17" s="10">
         <v>45583</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="F17" s="10">
+        <v>45583</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="I17" s="12"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
@@ -1234,13 +1261,21 @@
       <c r="C18" s="10">
         <v>45576</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="10">
+        <v>45576</v>
+      </c>
       <c r="E18" s="10">
         <v>45583</v>
       </c>
-      <c r="F18" s="10"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="F18" s="10">
+        <v>45583</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>23</v>
+      </c>
       <c r="I18" s="6"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
@@ -1265,19 +1300,25 @@
         <v>13</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="10">
         <v>45584</v>
       </c>
-      <c r="D19" s="7"/>
+      <c r="D19" s="10">
+        <v>45584</v>
+      </c>
       <c r="E19" s="10">
         <v>45591</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="6"/>
+      <c r="F19" s="10">
+        <v>45591</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="1"/>
@@ -1303,19 +1344,25 @@
         <v>14</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="10">
         <v>45584</v>
       </c>
-      <c r="D20" s="7"/>
+      <c r="D20" s="10">
+        <v>45584</v>
+      </c>
       <c r="E20" s="10">
         <v>45591</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="6"/>
+      <c r="F20" s="10">
+        <v>45591</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H20" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I20" s="6"/>
       <c r="J20" s="1"/>
@@ -1341,19 +1388,25 @@
         <v>15</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="10">
         <v>45584</v>
       </c>
-      <c r="D21" s="7"/>
+      <c r="D21" s="10">
+        <v>45584</v>
+      </c>
       <c r="E21" s="10">
         <v>45591</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="6"/>
+      <c r="F21" s="10">
+        <v>45591</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H21" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I21" s="6"/>
       <c r="J21" s="1"/>
@@ -1379,19 +1432,25 @@
         <v>16</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="10">
         <v>45584</v>
       </c>
-      <c r="D22" s="7"/>
+      <c r="D22" s="10">
+        <v>45584</v>
+      </c>
       <c r="E22" s="10">
         <v>45591</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="6"/>
+      <c r="F22" s="10">
+        <v>45591</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H22" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="1"/>
@@ -1417,19 +1476,25 @@
         <v>17</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C23" s="10">
         <v>45584</v>
       </c>
-      <c r="D23" s="7"/>
+      <c r="D23" s="10">
+        <v>45584</v>
+      </c>
       <c r="E23" s="10">
         <v>45591</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="6"/>
+      <c r="F23" s="10">
+        <v>45591</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H23" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="1"/>
@@ -1455,19 +1520,25 @@
         <v>18</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="10">
         <v>45592</v>
       </c>
-      <c r="D24" s="7"/>
+      <c r="D24" s="10">
+        <v>45592</v>
+      </c>
       <c r="E24" s="10">
         <v>45600</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="6"/>
+      <c r="F24" s="10">
+        <v>45600</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H24" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="1"/>
@@ -1493,19 +1564,25 @@
         <v>19</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="10">
         <v>45592</v>
       </c>
-      <c r="D25" s="7"/>
+      <c r="D25" s="10">
+        <v>45592</v>
+      </c>
       <c r="E25" s="10">
         <v>45600</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="6"/>
+      <c r="F25" s="10">
+        <v>45600</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H25" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="1"/>
@@ -1531,19 +1608,25 @@
         <v>20</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C26" s="10">
         <v>45592</v>
       </c>
-      <c r="D26" s="7"/>
+      <c r="D26" s="10">
+        <v>45592</v>
+      </c>
       <c r="E26" s="10">
         <v>45600</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="6"/>
+      <c r="F26" s="10">
+        <v>45600</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H26" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="1"/>
@@ -1569,19 +1652,25 @@
         <v>21</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="10">
         <v>45592</v>
       </c>
-      <c r="D27" s="7"/>
+      <c r="D27" s="10">
+        <v>45592</v>
+      </c>
       <c r="E27" s="10">
         <v>45600</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="6"/>
+      <c r="F27" s="10">
+        <v>45600</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H27" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="1"/>
@@ -1607,19 +1696,25 @@
         <v>22</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C28" s="10">
         <v>45592</v>
       </c>
-      <c r="D28" s="7"/>
+      <c r="D28" s="10">
+        <v>45592</v>
+      </c>
       <c r="E28" s="10">
         <v>45600</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="6"/>
+      <c r="F28" s="10">
+        <v>45600</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H28" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="1"/>
@@ -1645,17 +1740,23 @@
         <v>23</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="10">
         <v>45601</v>
       </c>
-      <c r="D29" s="7"/>
+      <c r="D29" s="10">
+        <v>45601</v>
+      </c>
       <c r="E29" s="10">
-        <v>45614</v>
+        <v>45616</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="6"/>
+      <c r="F29" s="10">
+        <v>45616</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H29" s="6" t="s">
         <v>11</v>
       </c>
@@ -1683,17 +1784,23 @@
         <v>24</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" s="10">
-        <v>45615</v>
+        <v>45617</v>
       </c>
-      <c r="D30" s="7"/>
+      <c r="D30" s="10">
+        <v>45617</v>
+      </c>
       <c r="E30" s="10">
-        <v>45629</v>
+        <v>45634</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="6"/>
+      <c r="F30" s="10">
+        <v>45634</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H30" s="6" t="s">
         <v>11</v>
       </c>
@@ -1721,17 +1828,23 @@
         <v>25</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C31" s="7">
-        <v>45630</v>
+        <v>45635</v>
       </c>
-      <c r="D31" s="7"/>
+      <c r="D31" s="7">
+        <v>45635</v>
+      </c>
       <c r="E31" s="7">
         <v>45637</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="6"/>
+      <c r="F31" s="7">
+        <v>45637</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H31" s="6" t="s">
         <v>11</v>
       </c>
@@ -1759,19 +1872,25 @@
         <v>26</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C32" s="7">
         <v>45638</v>
       </c>
-      <c r="D32" s="7"/>
+      <c r="D32" s="7">
+        <v>45638</v>
+      </c>
       <c r="E32" s="7">
-        <v>45639</v>
+        <v>45641</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="6"/>
+      <c r="F32" s="7">
+        <v>45641</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H32" s="6" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="I32" s="6"/>
       <c r="J32" s="1"/>
@@ -1800,15 +1919,23 @@
         <v>18</v>
       </c>
       <c r="C33" s="7">
-        <v>45640</v>
-      </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7">
         <v>45642</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
+      <c r="D33" s="7">
+        <v>45642</v>
+      </c>
+      <c r="E33" s="7">
+        <v>45643</v>
+      </c>
+      <c r="F33" s="7">
+        <v>45643</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>11</v>
+      </c>
       <c r="I33" s="6"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
@@ -1833,17 +1960,23 @@
         <v>28</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C34" s="7">
-        <v>45643</v>
-      </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7">
         <v>45644</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="6"/>
+      <c r="D34" s="7">
+        <v>45644</v>
+      </c>
+      <c r="E34" s="7">
+        <v>45648</v>
+      </c>
+      <c r="F34" s="7">
+        <v>45648</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="H34" s="6" t="s">
         <v>11</v>
       </c>

</xml_diff>